<commit_message>
Update 4 and 5 labs
</commit_message>
<xml_diff>
--- a/labs/lab5/task1/Pairwise.xlsx
+++ b/labs/lab5/task1/Pairwise.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Font</t>
   </si>
@@ -38,37 +38,58 @@
     <t>Size</t>
   </si>
   <si>
+    <t>Upline</t>
+  </si>
+  <si>
+    <t>Double Strikethrough</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Small caps</t>
+  </si>
+  <si>
+    <t>All caps</t>
+  </si>
+  <si>
+    <t>Align the height of characters</t>
+  </si>
+  <si>
     <t>Times new Roman</t>
   </si>
   <si>
+    <t>Uncheck</t>
+  </si>
+  <si>
     <t>Check</t>
   </si>
   <si>
-    <t>Uncheck</t>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Unckeck</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Roboto</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
   <si>
     <t>Red</t>
-  </si>
-  <si>
-    <t>Large</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Roboto</t>
-  </si>
-  <si>
-    <t>Small</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Green</t>
   </si>
   <si>
     <t>Blue</t>
@@ -428,13 +449,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,9 +467,15 @@
     <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="36.419678" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,502 +497,862 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2">
+        <v>100</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2">
+        <v>100</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2">
+        <v>50</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2">
+        <v>100</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2">
+        <v>50</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2">
+        <v>100</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="2">
+        <v>50</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="2" customFormat="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2">
+        <v>100</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="2" customFormat="1">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1">
+      <c r="I15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="2" customFormat="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="2">
+        <v>50</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="2">
+        <v>100</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="2" customFormat="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="2">
+        <v>50</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="2" customFormat="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="2">
+        <v>100</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="2" customFormat="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -973,25 +1360,43 @@
         <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="2" customFormat="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -999,25 +1404,43 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="2">
+        <v>50</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1025,25 +1448,43 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="2">
+        <v>100</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="2" customFormat="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1051,25 +1492,43 @@
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="2" customFormat="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1077,25 +1536,43 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="2">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1103,22 +1580,832 @@
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="2">
+        <v>100</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="2" customFormat="1">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="2" customFormat="1">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="2">
+        <v>50</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="2" customFormat="1">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="2">
+        <v>100</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="2" customFormat="1">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="2" customFormat="1">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="2">
+        <v>50</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="2" customFormat="1">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="2">
+        <v>100</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="2" customFormat="1">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="2">
+        <v>50</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="2" customFormat="1">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="2">
+        <v>100</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="2" customFormat="1">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="2" customFormat="1">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="2">
+        <v>50</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="2" customFormat="1">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="2">
+        <v>100</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="2" customFormat="1">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="2" customFormat="1">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="2">
+        <v>50</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="2" customFormat="1">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="2">
+        <v>100</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="2" customFormat="1">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="2" customFormat="1">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="2">
+        <v>50</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="2" customFormat="1">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="2">
+        <v>100</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>